<commit_message>
Updating Requirement Sheet [Draft]
</commit_message>
<xml_diff>
--- a/Documents/MTRN4230 Asst 2 Requirements Tracking Group L 170814.xlsx
+++ b/Documents/MTRN4230 Asst 2 Requirements Tracking Group L 170814.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ken\Documents\University\2017 - Semester 2\MTRN4230 Robotics\GITHUB\mtrn4230\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ken\Documents\University\2017 - Semester 2\MTRN4230 Robotics\GITHUB\mtrn4230\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
   <si>
     <t>Last updated</t>
   </si>
@@ -314,6 +314,30 @@
   </si>
   <si>
     <t>A</t>
+  </si>
+  <si>
+    <t>Everyone</t>
+  </si>
+  <si>
+    <t>Ken</t>
+  </si>
+  <si>
+    <t>Jay</t>
+  </si>
+  <si>
+    <t>Herman</t>
+  </si>
+  <si>
+    <t>Daniel, Herman, Ken</t>
+  </si>
+  <si>
+    <t>Ravi,Emtiazul,Jay</t>
+  </si>
+  <si>
+    <t>Undetermined</t>
+  </si>
+  <si>
+    <t>L</t>
   </si>
 </sst>
 </file>
@@ -812,7 +836,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H15" sqref="H15"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -820,9 +844,9 @@
     <col min="1" max="1" width="8.85546875" customWidth="1"/>
     <col min="2" max="2" width="8.42578125" customWidth="1"/>
     <col min="3" max="3" width="15.42578125" customWidth="1"/>
-    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="4" max="4" width="17.140625" customWidth="1"/>
     <col min="5" max="5" width="18.140625" customWidth="1"/>
-    <col min="6" max="6" width="7.5703125" customWidth="1"/>
+    <col min="6" max="6" width="40.28515625" customWidth="1"/>
     <col min="7" max="7" width="17" customWidth="1"/>
     <col min="8" max="8" width="74" customWidth="1"/>
     <col min="9" max="26" width="7.5703125" customWidth="1"/>
@@ -863,7 +887,7 @@
         <v>0</v>
       </c>
       <c r="B2" s="1">
-        <v>20170814</v>
+        <v>20170824</v>
       </c>
       <c r="C2" s="2"/>
       <c r="D2" s="2" t="s">
@@ -898,9 +922,13 @@
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="1"/>
+      <c r="B3" s="1" t="s">
+        <v>98</v>
+      </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
+      <c r="D3" s="2" t="s">
+        <v>104</v>
+      </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
       <c r="G3" s="3"/>
@@ -1073,7 +1101,9 @@
       <c r="D8" s="1">
         <v>20170814</v>
       </c>
-      <c r="E8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F8" s="2"/>
       <c r="G8" s="3" t="s">
         <v>16</v>
@@ -1113,7 +1143,9 @@
       <c r="D9" s="1">
         <v>20170814</v>
       </c>
-      <c r="E9" s="2"/>
+      <c r="E9" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F9" s="2"/>
       <c r="G9" s="3" t="s">
         <v>19</v>
@@ -1153,7 +1185,9 @@
       <c r="D10" s="1">
         <v>20170814</v>
       </c>
-      <c r="E10" s="2"/>
+      <c r="E10" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F10" s="2"/>
       <c r="G10" s="3" t="s">
         <v>22</v>
@@ -1193,7 +1227,9 @@
       <c r="D11" s="1">
         <v>20170814</v>
       </c>
-      <c r="E11" s="2"/>
+      <c r="E11" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F11" s="2"/>
       <c r="G11" s="3" t="s">
         <v>25</v>
@@ -1233,7 +1269,9 @@
       <c r="D12" s="1">
         <v>20170814</v>
       </c>
-      <c r="E12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="F12" s="2"/>
       <c r="G12" s="3" t="s">
         <v>28</v>
@@ -1273,7 +1311,9 @@
       <c r="D13" s="1">
         <v>20170814</v>
       </c>
-      <c r="E13" s="2"/>
+      <c r="E13" s="6" t="s">
+        <v>102</v>
+      </c>
       <c r="F13" s="2"/>
       <c r="G13" s="3" t="s">
         <v>31</v>
@@ -1313,7 +1353,9 @@
       <c r="D14" s="1">
         <v>20170814</v>
       </c>
-      <c r="E14" s="2"/>
+      <c r="E14" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F14" s="2"/>
       <c r="G14" s="3" t="s">
         <v>94</v>
@@ -1353,7 +1395,9 @@
       <c r="D15" s="1">
         <v>20170814</v>
       </c>
-      <c r="E15" s="2"/>
+      <c r="E15" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="F15" s="2"/>
       <c r="G15" s="3" t="s">
         <v>95</v>
@@ -1451,7 +1495,9 @@
       <c r="D18" s="1">
         <v>20170814</v>
       </c>
-      <c r="E18" s="2"/>
+      <c r="E18" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="F18" s="2"/>
       <c r="G18" s="3" t="s">
         <v>35</v>
@@ -1491,7 +1537,9 @@
       <c r="D19" s="1">
         <v>20170814</v>
       </c>
-      <c r="E19" s="2"/>
+      <c r="E19" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="F19" s="2"/>
       <c r="G19" s="3" t="s">
         <v>38</v>
@@ -1589,7 +1637,9 @@
       <c r="D22" s="1">
         <v>20170814</v>
       </c>
-      <c r="E22" s="2"/>
+      <c r="E22" s="6" t="s">
+        <v>101</v>
+      </c>
       <c r="F22" s="2"/>
       <c r="G22" s="3" t="s">
         <v>42</v>
@@ -1629,7 +1679,9 @@
       <c r="D23" s="1">
         <v>20170814</v>
       </c>
-      <c r="E23" s="2"/>
+      <c r="E23" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="F23" s="2"/>
       <c r="G23" s="3" t="s">
         <v>45</v>
@@ -1669,7 +1721,9 @@
       <c r="D24" s="1">
         <v>20170814</v>
       </c>
-      <c r="E24" s="2"/>
+      <c r="E24" s="2" t="s">
+        <v>101</v>
+      </c>
       <c r="F24" s="2"/>
       <c r="G24" s="3" t="s">
         <v>48</v>
@@ -1767,7 +1821,9 @@
       <c r="D27" s="1">
         <v>20170814</v>
       </c>
-      <c r="E27" s="2"/>
+      <c r="E27" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F27" s="2"/>
       <c r="G27" s="3" t="s">
         <v>52</v>
@@ -1807,7 +1863,9 @@
       <c r="D28" s="1">
         <v>20170814</v>
       </c>
-      <c r="E28" s="2"/>
+      <c r="E28" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F28" s="2"/>
       <c r="G28" s="3" t="s">
         <v>55</v>
@@ -1847,7 +1905,9 @@
       <c r="D29" s="1">
         <v>20170814</v>
       </c>
-      <c r="E29" s="2"/>
+      <c r="E29" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F29" s="2"/>
       <c r="G29" s="3" t="s">
         <v>58</v>
@@ -1887,7 +1947,9 @@
       <c r="D30" s="1">
         <v>20170814</v>
       </c>
-      <c r="E30" s="2"/>
+      <c r="E30" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F30" s="2"/>
       <c r="G30" s="3" t="s">
         <v>61</v>
@@ -1927,7 +1989,9 @@
       <c r="D31" s="1">
         <v>20170814</v>
       </c>
-      <c r="E31" s="2"/>
+      <c r="E31" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F31" s="2"/>
       <c r="G31" s="3" t="s">
         <v>64</v>
@@ -1967,7 +2031,9 @@
       <c r="D32" s="1">
         <v>20170814</v>
       </c>
-      <c r="E32" s="2"/>
+      <c r="E32" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F32" s="2"/>
       <c r="G32" s="3" t="s">
         <v>67</v>
@@ -2007,7 +2073,9 @@
       <c r="D33" s="1">
         <v>20170814</v>
       </c>
-      <c r="E33" s="2"/>
+      <c r="E33" s="6" t="s">
+        <v>103</v>
+      </c>
       <c r="F33" s="2"/>
       <c r="G33" s="3" t="s">
         <v>70</v>
@@ -2105,7 +2173,9 @@
       <c r="D36" s="1">
         <v>20170814</v>
       </c>
-      <c r="E36" s="2"/>
+      <c r="E36" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F36" s="2"/>
       <c r="G36" s="4" t="s">
         <v>72</v>
@@ -2145,7 +2215,9 @@
       <c r="D37" s="1">
         <v>20170814</v>
       </c>
-      <c r="E37" s="2"/>
+      <c r="E37" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F37" s="2"/>
       <c r="G37" s="4" t="s">
         <v>76</v>
@@ -2243,7 +2315,9 @@
       <c r="D40" s="1">
         <v>20170814</v>
       </c>
-      <c r="E40" s="2"/>
+      <c r="E40" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="F40" s="2"/>
       <c r="G40" s="3" t="s">
         <v>80</v>
@@ -2283,7 +2357,9 @@
       <c r="D41" s="1">
         <v>20170814</v>
       </c>
-      <c r="E41" s="2"/>
+      <c r="E41" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F41" s="2"/>
       <c r="G41" s="4" t="s">
         <v>82</v>
@@ -2323,7 +2399,9 @@
       <c r="D42" s="1">
         <v>20170814</v>
       </c>
-      <c r="E42" s="2"/>
+      <c r="E42" s="2" t="s">
+        <v>97</v>
+      </c>
       <c r="F42" s="2"/>
       <c r="G42" s="3" t="s">
         <v>84</v>

</xml_diff>

<commit_message>
Updated Tasks Tracking Sheet
</commit_message>
<xml_diff>
--- a/Documents/MTRN4230 Asst 2 Requirements Tracking Group L 170814.xlsx
+++ b/Documents/MTRN4230 Asst 2 Requirements Tracking Group L 170814.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="17726"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ken\Documents\University\2017 - Semester 2\MTRN4230 Robotics\GITHUB\mtrn4230\Documents\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel Castillo\Documents\GitHub\mtrn4230\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -18,12 +18,12 @@
   <definedNames>
     <definedName name="Stati">Working!$A$3:$A$5</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="152" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="106">
   <si>
     <t>Last updated</t>
   </si>
@@ -328,22 +328,25 @@
     <t>Herman</t>
   </si>
   <si>
-    <t>Daniel, Herman, Ken</t>
+    <t>L</t>
   </si>
   <si>
-    <t>Ravi,Emtiazul,Jay</t>
+    <t>Daniel</t>
   </si>
   <si>
-    <t>Undetermined</t>
+    <t>Ravi</t>
   </si>
   <si>
-    <t>L</t>
+    <t xml:space="preserve">Ken </t>
+  </si>
+  <si>
+    <t>Emtiazul</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -400,7 +403,3437 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
+  <dxfs count="252">
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFFC000"/>
+          <bgColor rgb="FFFFC000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FF92D050"/>
+          <bgColor rgb="FF92D050"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor rgb="FFFF0000"/>
+          <bgColor rgb="FFFF0000"/>
+        </patternFill>
+      </fill>
+      <border>
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -588,23 +4021,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -640,23 +4056,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -835,8 +4234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Z1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" topLeftCell="C9" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="15.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -927,7 +4326,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="D3" s="2" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E3" s="2"/>
       <c r="F3" s="2"/>
@@ -1095,16 +4494,18 @@
       <c r="B8" s="2">
         <v>2</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>15</v>
+      <c r="C8" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D8" s="1">
         <v>20170814</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="G8" s="3" t="s">
         <v>16</v>
       </c>
@@ -1137,16 +4538,18 @@
       <c r="B9" s="2">
         <v>3</v>
       </c>
-      <c r="C9" s="2" t="s">
-        <v>15</v>
+      <c r="C9" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D9" s="1">
         <v>20170814</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="G9" s="3" t="s">
         <v>19</v>
       </c>
@@ -1179,16 +4582,18 @@
       <c r="B10" s="2">
         <v>1</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>15</v>
+      <c r="C10" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D10" s="1">
         <v>20170814</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
-      <c r="F10" s="2"/>
+      <c r="F10" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="G10" s="3" t="s">
         <v>22</v>
       </c>
@@ -1221,16 +4626,16 @@
       <c r="B11" s="2">
         <v>1</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="C11" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D11" s="1">
         <v>20170814</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
-      <c r="F11" s="2"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="3" t="s">
         <v>25</v>
       </c>
@@ -1263,16 +4668,18 @@
       <c r="B12" s="2">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="s">
-        <v>15</v>
+      <c r="C12" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D12" s="1">
         <v>20170814</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="G12" s="3" t="s">
         <v>28</v>
       </c>
@@ -1305,16 +4712,18 @@
       <c r="B13" s="2">
         <v>2</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>15</v>
+      <c r="C13" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D13" s="1">
         <v>20170814</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="G13" s="3" t="s">
         <v>31</v>
       </c>
@@ -1347,16 +4756,18 @@
       <c r="B14" s="1">
         <v>3</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>15</v>
+      <c r="C14" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D14" s="1">
         <v>20170814</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
-      <c r="F14" s="2"/>
+      <c r="F14" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="G14" s="3" t="s">
         <v>94</v>
       </c>
@@ -1389,8 +4800,8 @@
       <c r="B15" s="2">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>15</v>
+      <c r="C15" s="6" t="s">
+        <v>87</v>
       </c>
       <c r="D15" s="1">
         <v>20170814</v>
@@ -1398,7 +4809,9 @@
       <c r="E15" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="F15" s="2"/>
+      <c r="F15" s="6" t="s">
+        <v>99</v>
+      </c>
       <c r="G15" s="3" t="s">
         <v>95</v>
       </c>
@@ -1489,14 +4902,14 @@
       <c r="B18" s="2">
         <v>1</v>
       </c>
-      <c r="C18" s="2" t="s">
+      <c r="C18" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D18" s="1">
         <v>20170814</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F18" s="2"/>
       <c r="G18" s="3" t="s">
@@ -1531,16 +4944,18 @@
       <c r="B19" s="2">
         <v>1</v>
       </c>
-      <c r="C19" s="2" t="s">
-        <v>15</v>
+      <c r="C19" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D19" s="1">
         <v>20170814</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
-      <c r="F19" s="2"/>
+      <c r="F19" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="G19" s="3" t="s">
         <v>38</v>
       </c>
@@ -1631,14 +5046,14 @@
       <c r="B22" s="2">
         <v>1</v>
       </c>
-      <c r="C22" s="2" t="s">
+      <c r="C22" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D22" s="1">
         <v>20170814</v>
       </c>
       <c r="E22" s="6" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="F22" s="2"/>
       <c r="G22" s="3" t="s">
@@ -1673,8 +5088,8 @@
       <c r="B23" s="2">
         <v>2</v>
       </c>
-      <c r="C23" s="2" t="s">
-        <v>15</v>
+      <c r="C23" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D23" s="1">
         <v>20170814</v>
@@ -1682,7 +5097,9 @@
       <c r="E23" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="F23" s="2"/>
+      <c r="F23" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="G23" s="3" t="s">
         <v>45</v>
       </c>
@@ -1715,16 +5132,18 @@
       <c r="B24" s="2">
         <v>2</v>
       </c>
-      <c r="C24" s="2" t="s">
-        <v>15</v>
+      <c r="C24" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D24" s="1">
         <v>20170814</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
-      <c r="F24" s="2"/>
+      <c r="F24" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G24" s="3" t="s">
         <v>48</v>
       </c>
@@ -1815,16 +5234,18 @@
       <c r="B27" s="2">
         <v>2</v>
       </c>
-      <c r="C27" s="2" t="s">
-        <v>15</v>
+      <c r="C27" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D27" s="1">
         <v>20170814</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
-      <c r="F27" s="2"/>
+      <c r="F27" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G27" s="3" t="s">
         <v>52</v>
       </c>
@@ -1857,16 +5278,18 @@
       <c r="B28" s="2">
         <v>5</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>15</v>
+      <c r="C28" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D28" s="1">
         <v>20170814</v>
       </c>
       <c r="E28" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
-      <c r="F28" s="2"/>
+      <c r="F28" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G28" s="3" t="s">
         <v>55</v>
       </c>
@@ -1899,16 +5322,18 @@
       <c r="B29" s="2">
         <v>0</v>
       </c>
-      <c r="C29" s="2" t="s">
-        <v>15</v>
+      <c r="C29" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D29" s="1">
         <v>20170814</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
-      <c r="F29" s="2"/>
+      <c r="F29" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="G29" s="3" t="s">
         <v>58</v>
       </c>
@@ -1941,16 +5366,18 @@
       <c r="B30" s="2">
         <v>1</v>
       </c>
-      <c r="C30" s="2" t="s">
-        <v>15</v>
+      <c r="C30" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D30" s="1">
         <v>20170814</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
-      <c r="F30" s="2"/>
+      <c r="F30" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G30" s="3" t="s">
         <v>61</v>
       </c>
@@ -1983,16 +5410,18 @@
       <c r="B31" s="2">
         <v>1</v>
       </c>
-      <c r="C31" s="2" t="s">
-        <v>15</v>
+      <c r="C31" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D31" s="1">
         <v>20170814</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
-      <c r="F31" s="2"/>
+      <c r="F31" s="2" t="s">
+        <v>102</v>
+      </c>
       <c r="G31" s="3" t="s">
         <v>64</v>
       </c>
@@ -2025,14 +5454,14 @@
       <c r="B32" s="2">
         <v>1</v>
       </c>
-      <c r="C32" s="2" t="s">
+      <c r="C32" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D32" s="1">
         <v>20170814</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F32" s="2"/>
       <c r="G32" s="3" t="s">
@@ -2067,14 +5496,14 @@
       <c r="B33" s="2">
         <v>2</v>
       </c>
-      <c r="C33" s="2" t="s">
+      <c r="C33" s="6" t="s">
         <v>15</v>
       </c>
       <c r="D33" s="1">
         <v>20170814</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="F33" s="2"/>
       <c r="G33" s="3" t="s">
@@ -2168,7 +5597,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="2" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D36" s="1">
         <v>20170814</v>
@@ -2176,7 +5605,9 @@
       <c r="E36" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F36" s="2"/>
+      <c r="F36" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="G36" s="4" t="s">
         <v>72</v>
       </c>
@@ -2209,8 +5640,8 @@
       <c r="B37" s="2">
         <v>1</v>
       </c>
-      <c r="C37" s="2" t="s">
-        <v>15</v>
+      <c r="C37" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D37" s="1">
         <v>20170814</v>
@@ -2218,7 +5649,9 @@
       <c r="E37" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F37" s="2"/>
+      <c r="F37" s="6" t="s">
+        <v>97</v>
+      </c>
       <c r="G37" s="4" t="s">
         <v>76</v>
       </c>
@@ -2309,8 +5742,8 @@
       <c r="B40" s="2">
         <v>2</v>
       </c>
-      <c r="C40" s="2" t="s">
-        <v>15</v>
+      <c r="C40" s="6" t="s">
+        <v>88</v>
       </c>
       <c r="D40" s="1">
         <v>20170814</v>
@@ -2318,7 +5751,9 @@
       <c r="E40" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="F40" s="2"/>
+      <c r="F40" s="2" t="s">
+        <v>98</v>
+      </c>
       <c r="G40" s="3" t="s">
         <v>80</v>
       </c>
@@ -2352,7 +5787,7 @@
         <v>2</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D41" s="1">
         <v>20170814</v>
@@ -2360,7 +5795,9 @@
       <c r="E41" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F41" s="2"/>
+      <c r="F41" s="6" t="s">
+        <v>105</v>
+      </c>
       <c r="G41" s="4" t="s">
         <v>82</v>
       </c>
@@ -2394,7 +5831,7 @@
         <v>3</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>15</v>
+        <v>87</v>
       </c>
       <c r="D42" s="1">
         <v>20170814</v>
@@ -2402,7 +5839,9 @@
       <c r="E42" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="F42" s="2"/>
+      <c r="F42" s="2" t="s">
+        <v>105</v>
+      </c>
       <c r="G42" s="3" t="s">
         <v>84</v>
       </c>
@@ -29258,43 +32697,338 @@
       <c r="Z1000" s="2"/>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="C41:C52 C25:C26 C20:C21 C34:C36 C14:C17">
+    <cfRule type="containsText" dxfId="250" priority="130" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C47))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41:C52 C25:C26 C20:C21 C34:C36 C14:C17">
+    <cfRule type="containsText" dxfId="249" priority="131" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C47))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C41:C52 C34:C36 C25:C26 C20:C21 C14:C17">
+    <cfRule type="containsText" dxfId="248" priority="132" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C14))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C39">
+    <cfRule type="containsText" dxfId="247" priority="133" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C38))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C39">
+    <cfRule type="containsText" dxfId="246" priority="134" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C38))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C38:C39">
+    <cfRule type="containsText" dxfId="245" priority="135" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C38))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="163" priority="75" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C37))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="161" priority="76" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C37))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37">
+    <cfRule type="containsText" dxfId="159" priority="77" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C37))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="containsText" dxfId="119" priority="55" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="containsText" dxfId="117" priority="56" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C27">
+    <cfRule type="containsText" dxfId="115" priority="57" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C27))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="containsText" dxfId="113" priority="52" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="containsText" dxfId="111" priority="53" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C28">
+    <cfRule type="containsText" dxfId="109" priority="54" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C28))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="107" priority="49" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="105" priority="50" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C29">
+    <cfRule type="containsText" dxfId="103" priority="51" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C29))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="containsText" dxfId="101" priority="46" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="containsText" dxfId="99" priority="47" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C30">
+    <cfRule type="containsText" dxfId="97" priority="48" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C30))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="containsText" dxfId="95" priority="43" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="containsText" dxfId="93" priority="44" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C31">
+    <cfRule type="containsText" dxfId="91" priority="45" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C31))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="containsText" dxfId="89" priority="40" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="containsText" dxfId="87" priority="41" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C33">
+    <cfRule type="containsText" dxfId="85" priority="42" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C33))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="83" priority="37" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="81" priority="38" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C32">
+    <cfRule type="containsText" dxfId="79" priority="39" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C32))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="containsText" dxfId="77" priority="34" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="containsText" dxfId="75" priority="35" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C22">
+    <cfRule type="containsText" dxfId="73" priority="36" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C22))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="containsText" dxfId="71" priority="31" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="containsText" dxfId="69" priority="32" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C23">
+    <cfRule type="containsText" dxfId="67" priority="33" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C23))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="65" priority="28" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="63" priority="29" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C24">
+    <cfRule type="containsText" dxfId="61" priority="30" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C24))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="59" priority="25" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="57" priority="26" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C19">
+    <cfRule type="containsText" dxfId="55" priority="27" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C19))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsText" dxfId="53" priority="22" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsText" dxfId="51" priority="23" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C13">
+    <cfRule type="containsText" dxfId="49" priority="24" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C13))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="47" priority="19" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="45" priority="20" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C12">
+    <cfRule type="containsText" dxfId="43" priority="21" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C12))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="41" priority="16" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="39" priority="17" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C9">
+    <cfRule type="containsText" dxfId="37" priority="18" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C9))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="containsText" dxfId="35" priority="13" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="containsText" dxfId="33" priority="14" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10">
+    <cfRule type="containsText" dxfId="31" priority="15" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C10))))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <conditionalFormatting sqref="C8">
-    <cfRule type="containsText" dxfId="6" priority="1" operator="containsText" text="Pass.">
+    <cfRule type="containsText" dxfId="29" priority="10" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C8))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="27" priority="11" operator="containsText" text="Pass.">
       <formula>NOT(ISERROR(SEARCH(("Pass."),(C8))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C52 C8:C36">
-    <cfRule type="containsText" dxfId="5" priority="2" operator="containsText" text="Fail. Solution unknown.">
-      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C41))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C41:C52 C8:C36">
-    <cfRule type="containsText" dxfId="4" priority="3" operator="containsText" text="Pass.">
-      <formula>NOT(ISERROR(SEARCH(("Pass."),(C41))))</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="C8:C31 C41:C52 C34:C36">
-    <cfRule type="containsText" dxfId="3" priority="4" operator="containsText" text="Fail. Solution known.">
+  <conditionalFormatting sqref="C8">
+    <cfRule type="containsText" dxfId="25" priority="12" operator="containsText" text="Fail. Solution known.">
       <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C8))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C40">
-    <cfRule type="containsText" dxfId="2" priority="5" operator="containsText" text="Fail. Solution unknown.">
-      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C37))))</formula>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="23" priority="7" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C11))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C40">
-    <cfRule type="containsText" dxfId="1" priority="6" operator="containsText" text="Pass.">
-      <formula>NOT(ISERROR(SEARCH(("Pass."),(C37))))</formula>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="21" priority="8" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C11))))</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C38:C40">
-    <cfRule type="containsText" dxfId="0" priority="7" operator="containsText" text="Fail. Solution known.">
-      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C38))))</formula>
+  <conditionalFormatting sqref="C11">
+    <cfRule type="containsText" dxfId="19" priority="9" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C11))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="11" priority="4" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="9" priority="5" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C18">
+    <cfRule type="containsText" dxfId="7" priority="6" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C18))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="5" priority="1" operator="containsText" text="Fail. Solution unknown.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution unknown."),(C40))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="Pass.">
+      <formula>NOT(ISERROR(SEARCH(("Pass."),(C40))))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C40">
+    <cfRule type="containsText" dxfId="1" priority="3" operator="containsText" text="Fail. Solution known.">
+      <formula>NOT(ISERROR(SEARCH(("Fail. Solution known."),(C40))))</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C8:C13 C16:C18 C20:C23 C25:C31 C34:C36 C38:C52">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" sqref="C8:C52">
       <formula1>Stati</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>